<commit_message>
Milestone: DRR updated with ecology, region, zone
</commit_message>
<xml_diff>
--- a/desinventar/match_muni_DRR_to_DES_edited_manually.xlsx
+++ b/desinventar/match_muni_DRR_to_DES_edited_manually.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29010" windowHeight="12240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29010" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5080,7 +5080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E746"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D659" sqref="D659"/>
     </sheetView>
   </sheetViews>
@@ -17777,7 +17777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>